<commit_message>
progress in presentation templates
</commit_message>
<xml_diff>
--- a/information/modelo_relacional_cineworld.xlsx
+++ b/information/modelo_relacional_cineworld.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Escritorio\Proyectos-personales\cineworld\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Escritorio\Proyectos-personales\cineworld\information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1919D35-A62C-4BE4-B6C3-60516FF82E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8988C675-C98A-478F-B8BD-3762550589C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="42">
   <si>
     <t>Teatro</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>NN,ND</t>
+  </si>
+  <si>
+    <t>horarios</t>
   </si>
 </sst>
 </file>
@@ -189,10 +192,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B6:AF15"/>
+  <dimension ref="B6:AF30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -781,6 +785,51 @@
       </c>
       <c r="R15" s="2"/>
     </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" s="3">
+        <v>4.8611111111111112E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" s="3">
+        <v>6.9444444444444434E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="3">
+        <v>0.15972222222222224</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" s="3">
+        <v>0.18055555555555555</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" s="3">
+        <v>0.27083333333333331</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29" s="3">
+        <v>0.38194444444444442</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B30" s="3">
+        <v>0.40277777777777773</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>